<commit_message>
new version built without dash
</commit_message>
<xml_diff>
--- a/entities.xlsx
+++ b/entities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrychapman/Documents/Analysis Projects/brandsDashboard/TopBrandsDashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrychapman/Documents/Analysis Projects/newBrandsDashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0BD2CE-34B5-2D4E-97AA-711865940647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94876B56-CC35-524D-9409-DF37CF1C2836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="760" windowWidth="35740" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newEntities" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="412">
   <si>
     <t>EntityName</t>
   </si>
@@ -1226,6 +1226,36 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Sephora</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>Food + Beverage</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Fashion</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Consumer Goods</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Consulting</t>
   </si>
 </sst>
 </file>
@@ -2084,1536 +2114,1840 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
+        <v>404</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10" t="s">
+        <v>405</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
       <c r="B11" t="s">
+        <v>406</v>
+      </c>
+      <c r="C11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12" t="s">
+        <v>404</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
+        <v>403</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="B14" t="s">
+        <v>403</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>40</v>
       </c>
       <c r="B15" t="s">
+        <v>406</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
+        <v>407</v>
+      </c>
+      <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>46</v>
       </c>
       <c r="B17" t="s">
+        <v>407</v>
+      </c>
+      <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
       <c r="B18" t="s">
+        <v>407</v>
+      </c>
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>52</v>
       </c>
       <c r="B19" t="s">
+        <v>407</v>
+      </c>
+      <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>55</v>
       </c>
       <c r="B20" t="s">
+        <v>407</v>
+      </c>
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>58</v>
       </c>
       <c r="B21" t="s">
+        <v>407</v>
+      </c>
+      <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>61</v>
       </c>
       <c r="B22" t="s">
+        <v>407</v>
+      </c>
+      <c r="C22" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>64</v>
       </c>
       <c r="B23" t="s">
+        <v>406</v>
+      </c>
+      <c r="C23" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>67</v>
       </c>
       <c r="B24" t="s">
+        <v>406</v>
+      </c>
+      <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>70</v>
       </c>
       <c r="B25" t="s">
+        <v>408</v>
+      </c>
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>73</v>
       </c>
       <c r="B26" t="s">
+        <v>407</v>
+      </c>
+      <c r="C26" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>76</v>
       </c>
       <c r="B27" t="s">
+        <v>403</v>
+      </c>
+      <c r="C27" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>79</v>
       </c>
       <c r="B28" t="s">
+        <v>408</v>
+      </c>
+      <c r="C28" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
       <c r="B29" t="s">
+        <v>409</v>
+      </c>
+      <c r="C29" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
       <c r="B30" t="s">
+        <v>410</v>
+      </c>
+      <c r="C30" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
       <c r="B31" t="s">
+        <v>406</v>
+      </c>
+      <c r="C31" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>91</v>
       </c>
       <c r="B32" t="s">
+        <v>411</v>
+      </c>
+      <c r="C32" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>94</v>
       </c>
       <c r="B33" t="s">
+        <v>404</v>
+      </c>
+      <c r="C33" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>97</v>
       </c>
       <c r="B34" t="s">
+        <v>407</v>
+      </c>
+      <c r="C34" t="s">
         <v>233</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>99</v>
       </c>
       <c r="B35" t="s">
+        <v>408</v>
+      </c>
+      <c r="C35" t="s">
         <v>234</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>101</v>
       </c>
       <c r="B36" t="s">
+        <v>403</v>
+      </c>
+      <c r="C36" t="s">
         <v>235</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>103</v>
       </c>
       <c r="B37" t="s">
+        <v>407</v>
+      </c>
+      <c r="C37" t="s">
         <v>236</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>105</v>
       </c>
       <c r="B38" t="s">
+        <v>407</v>
+      </c>
+      <c r="C38" t="s">
         <v>237</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>107</v>
       </c>
       <c r="B39" t="s">
+        <v>408</v>
+      </c>
+      <c r="C39" t="s">
         <v>238</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>109</v>
       </c>
       <c r="B40" t="s">
+        <v>405</v>
+      </c>
+      <c r="C40" t="s">
         <v>239</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>111</v>
       </c>
       <c r="B41" t="s">
+        <v>405</v>
+      </c>
+      <c r="C41" t="s">
         <v>240</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>113</v>
       </c>
       <c r="B42" t="s">
+        <v>408</v>
+      </c>
+      <c r="C42" t="s">
         <v>241</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>115</v>
       </c>
       <c r="B43" t="s">
+        <v>406</v>
+      </c>
+      <c r="C43" t="s">
         <v>242</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>117</v>
       </c>
       <c r="B44" t="s">
+        <v>408</v>
+      </c>
+      <c r="C44" t="s">
         <v>243</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>118</v>
       </c>
       <c r="B45" t="s">
+        <v>404</v>
+      </c>
+      <c r="C45" t="s">
         <v>244</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>120</v>
       </c>
       <c r="B46" t="s">
+        <v>404</v>
+      </c>
+      <c r="C46" t="s">
         <v>245</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>122</v>
       </c>
       <c r="B47" t="s">
+        <v>403</v>
+      </c>
+      <c r="C47" t="s">
         <v>246</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>124</v>
       </c>
       <c r="B48" t="s">
+        <v>406</v>
+      </c>
+      <c r="C48" t="s">
         <v>247</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>126</v>
       </c>
       <c r="B49" t="s">
+        <v>403</v>
+      </c>
+      <c r="C49" t="s">
         <v>248</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>127</v>
       </c>
       <c r="B50" t="s">
+        <v>408</v>
+      </c>
+      <c r="C50" t="s">
         <v>249</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>129</v>
       </c>
       <c r="B51" t="s">
+        <v>403</v>
+      </c>
+      <c r="C51" t="s">
         <v>250</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>131</v>
       </c>
       <c r="B52" t="s">
+        <v>404</v>
+      </c>
+      <c r="C52" t="s">
         <v>251</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>133</v>
       </c>
       <c r="B53" t="s">
+        <v>409</v>
+      </c>
+      <c r="C53" t="s">
         <v>252</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>354</v>
       </c>
       <c r="B54" t="s">
+        <v>403</v>
+      </c>
+      <c r="C54" t="s">
         <v>253</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>135</v>
       </c>
       <c r="B55" t="s">
+        <v>407</v>
+      </c>
+      <c r="C55" t="s">
         <v>254</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>137</v>
       </c>
       <c r="B56" t="s">
+        <v>407</v>
+      </c>
+      <c r="C56" t="s">
         <v>255</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>138</v>
       </c>
       <c r="B57" t="s">
+        <v>406</v>
+      </c>
+      <c r="C57" t="s">
         <v>256</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>140</v>
       </c>
       <c r="B58" t="s">
+        <v>408</v>
+      </c>
+      <c r="C58" t="s">
         <v>257</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>142</v>
       </c>
       <c r="B59" t="s">
+        <v>409</v>
+      </c>
+      <c r="C59" t="s">
         <v>258</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>144</v>
       </c>
       <c r="B60" t="s">
+        <v>407</v>
+      </c>
+      <c r="C60" t="s">
         <v>259</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>146</v>
       </c>
       <c r="B61" t="s">
+        <v>407</v>
+      </c>
+      <c r="C61" t="s">
         <v>260</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>148</v>
       </c>
       <c r="B62" t="s">
+        <v>403</v>
+      </c>
+      <c r="C62" t="s">
         <v>261</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>150</v>
       </c>
       <c r="B63" t="s">
+        <v>407</v>
+      </c>
+      <c r="C63" t="s">
         <v>262</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>152</v>
       </c>
       <c r="B64" t="s">
+        <v>409</v>
+      </c>
+      <c r="C64" t="s">
         <v>263</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>154</v>
       </c>
       <c r="B65" t="s">
+        <v>404</v>
+      </c>
+      <c r="C65" t="s">
         <v>264</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>156</v>
       </c>
       <c r="B66" t="s">
+        <v>408</v>
+      </c>
+      <c r="C66" t="s">
         <v>265</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>158</v>
       </c>
       <c r="B67" t="s">
+        <v>408</v>
+      </c>
+      <c r="C67" t="s">
         <v>266</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>160</v>
       </c>
       <c r="B68" t="s">
+        <v>404</v>
+      </c>
+      <c r="C68" t="s">
         <v>267</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>162</v>
       </c>
       <c r="B69" t="s">
+        <v>405</v>
+      </c>
+      <c r="C69" t="s">
         <v>268</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>164</v>
       </c>
       <c r="B70" t="s">
+        <v>407</v>
+      </c>
+      <c r="C70" t="s">
         <v>269</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>166</v>
       </c>
       <c r="B71" t="s">
+        <v>407</v>
+      </c>
+      <c r="C71" t="s">
         <v>270</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>168</v>
       </c>
       <c r="B72" t="s">
+        <v>409</v>
+      </c>
+      <c r="C72" t="s">
         <v>271</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>170</v>
       </c>
       <c r="B73" t="s">
+        <v>409</v>
+      </c>
+      <c r="C73" t="s">
         <v>272</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>172</v>
       </c>
       <c r="B74" t="s">
+        <v>404</v>
+      </c>
+      <c r="C74" t="s">
         <v>273</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>174</v>
       </c>
       <c r="B75" t="s">
+        <v>406</v>
+      </c>
+      <c r="C75" t="s">
         <v>274</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>176</v>
       </c>
       <c r="B76" t="s">
+        <v>403</v>
+      </c>
+      <c r="C76" t="s">
         <v>275</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>178</v>
       </c>
       <c r="B77" t="s">
+        <v>408</v>
+      </c>
+      <c r="C77" t="s">
         <v>276</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>180</v>
       </c>
       <c r="B78" t="s">
+        <v>406</v>
+      </c>
+      <c r="C78" t="s">
         <v>277</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>181</v>
       </c>
       <c r="B79" t="s">
+        <v>404</v>
+      </c>
+      <c r="C79" t="s">
         <v>278</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>183</v>
       </c>
       <c r="B80" t="s">
+        <v>410</v>
+      </c>
+      <c r="C80" t="s">
         <v>279</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>185</v>
       </c>
       <c r="B81" t="s">
+        <v>404</v>
+      </c>
+      <c r="C81" t="s">
         <v>280</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>187</v>
       </c>
       <c r="B82" t="s">
+        <v>407</v>
+      </c>
+      <c r="C82" t="s">
         <v>281</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>189</v>
       </c>
       <c r="B83" t="s">
+        <v>410</v>
+      </c>
+      <c r="C83" t="s">
         <v>282</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>191</v>
       </c>
       <c r="B84" t="s">
+        <v>403</v>
+      </c>
+      <c r="C84" t="s">
         <v>283</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>193</v>
       </c>
       <c r="B85" t="s">
+        <v>407</v>
+      </c>
+      <c r="C85" t="s">
         <v>284</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>195</v>
       </c>
       <c r="B86" t="s">
+        <v>404</v>
+      </c>
+      <c r="C86" t="s">
         <v>285</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>197</v>
       </c>
       <c r="B87" t="s">
+        <v>407</v>
+      </c>
+      <c r="C87" t="s">
         <v>286</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>199</v>
       </c>
       <c r="B88" t="s">
+        <v>403</v>
+      </c>
+      <c r="C88" t="s">
         <v>287</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>388</v>
       </c>
       <c r="B89" t="s">
+        <v>406</v>
+      </c>
+      <c r="C89" t="s">
         <v>288</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>202</v>
       </c>
       <c r="B90" t="s">
+        <v>406</v>
+      </c>
+      <c r="C90" t="s">
         <v>289</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>204</v>
       </c>
       <c r="B91" t="s">
+        <v>407</v>
+      </c>
+      <c r="C91" t="s">
         <v>290</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>206</v>
       </c>
       <c r="B92" t="s">
+        <v>407</v>
+      </c>
+      <c r="C92" t="s">
         <v>291</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>208</v>
       </c>
       <c r="B93" t="s">
+        <v>409</v>
+      </c>
+      <c r="C93" t="s">
         <v>292</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>210</v>
       </c>
       <c r="B94" t="s">
+        <v>404</v>
+      </c>
+      <c r="C94" t="s">
         <v>293</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>212</v>
       </c>
       <c r="B95" t="s">
+        <v>404</v>
+      </c>
+      <c r="C95" t="s">
         <v>294</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>214</v>
       </c>
       <c r="B96" t="s">
+        <v>404</v>
+      </c>
+      <c r="C96" t="s">
         <v>295</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>216</v>
       </c>
       <c r="B97" t="s">
+        <v>406</v>
+      </c>
+      <c r="C97" t="s">
         <v>296</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>218</v>
       </c>
       <c r="B98" t="s">
+        <v>407</v>
+      </c>
+      <c r="C98" t="s">
         <v>297</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>220</v>
       </c>
       <c r="B99" t="s">
+        <v>403</v>
+      </c>
+      <c r="C99" t="s">
         <v>298</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>222</v>
       </c>
       <c r="B100" t="s">
+        <v>403</v>
+      </c>
+      <c r="C100" t="s">
         <v>299</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>224</v>
       </c>
       <c r="B101" t="s">
+        <v>406</v>
+      </c>
+      <c r="C101" t="s">
         <v>300</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>225</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{D12F1D2D-4B1F-9442-8230-BA093CCDA23F}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{FA3024EF-FFBD-684D-9906-53225CA54BB7}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{4FE93F76-11C2-634E-B1BA-33CD6EED3C4F}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{0DE70282-1533-FB4C-B78F-7BE0837CF03F}"/>
-    <hyperlink ref="C11" r:id="rId5" xr:uid="{2FE01F9A-75C7-EE45-9469-1989FC2664C1}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{5C5E2DBC-A8AD-2844-9409-F9591E3DA727}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{B2A6DD76-F50B-864A-BCA1-15F8CD8AD2F7}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{38D8F804-B45A-6F41-AB35-55FFD71423C7}"/>
-    <hyperlink ref="C7" r:id="rId9" xr:uid="{3184A6BA-4C96-754E-B82D-4FF6352DAC7C}"/>
-    <hyperlink ref="C6" r:id="rId10" xr:uid="{3EEA19BB-BEFA-E041-A042-A84DECF94176}"/>
-    <hyperlink ref="C5" r:id="rId11" xr:uid="{0C3C1D74-1886-E948-8479-D03A38A04087}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{0D88BE8D-FCF7-3040-8284-06EB8E532A21}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{B177BDD6-35CA-AF4A-806D-E1566D9F25BB}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{D5461290-BDB0-4B4C-AC07-7BBEF6892BB5}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{484B8704-496B-2E48-885A-5472E9141AD4}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{EFFBA2DD-F5C7-4D42-8006-C5DB783D84E1}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{06E602B6-AA16-B448-BC4D-18D32CD932C7}"/>
-    <hyperlink ref="C27" r:id="rId18" xr:uid="{CA03CEA7-D903-0B47-BD15-0E012F5A8C55}"/>
-    <hyperlink ref="C26" r:id="rId19" xr:uid="{3507CF5C-F543-0F43-BEB0-DCA754D009BF}"/>
-    <hyperlink ref="C24" r:id="rId20" xr:uid="{4C82D90D-8FD6-2040-A1F0-96089A16509F}"/>
-    <hyperlink ref="C25" r:id="rId21" xr:uid="{32EB20C6-DC11-5040-B11B-6DCD9C5CDDA2}"/>
-    <hyperlink ref="C23" r:id="rId22" xr:uid="{3287F51F-E3CA-284E-8EBB-980F59767731}"/>
-    <hyperlink ref="C22" r:id="rId23" xr:uid="{571A85DD-AD55-6E4C-AABC-2F061989418E}"/>
-    <hyperlink ref="C21" r:id="rId24" xr:uid="{3E840ED0-DB72-3D40-8F7A-7A636A18CFE2}"/>
-    <hyperlink ref="C20" r:id="rId25" xr:uid="{6B54AEE2-013B-4C44-83D0-7ACEA638D760}"/>
-    <hyperlink ref="C19" r:id="rId26" xr:uid="{E166F943-AD05-C644-ADFA-E6EABF1F4DD6}"/>
-    <hyperlink ref="C28" r:id="rId27" xr:uid="{A87368AC-9E4A-C040-985C-E474B7165AC2}"/>
-    <hyperlink ref="C30" r:id="rId28" xr:uid="{0693A7AB-A5CC-CE44-A0A5-672D8C5E5CCB}"/>
-    <hyperlink ref="C29" r:id="rId29" xr:uid="{DB2CBE5D-C54C-9C4A-98CC-19C8994A1194}"/>
-    <hyperlink ref="C31" r:id="rId30" xr:uid="{6B30E3AF-1CF1-574A-B9FA-AA21C36DA4A4}"/>
-    <hyperlink ref="C32" r:id="rId31" xr:uid="{7103085F-DD81-3945-863D-D5FB32BDB2E1}"/>
-    <hyperlink ref="C33" r:id="rId32" xr:uid="{9D293948-3F61-6B42-A230-7F5AEC69950B}"/>
-    <hyperlink ref="C34" r:id="rId33" xr:uid="{274CB73F-F748-3E4C-87D9-3A18C2381AB8}"/>
-    <hyperlink ref="C36" r:id="rId34" xr:uid="{98178744-49F4-BE47-83D0-177CB7DD8461}"/>
-    <hyperlink ref="C35" r:id="rId35" xr:uid="{E2F229ED-615E-7F47-9665-16C479E0930F}"/>
-    <hyperlink ref="C37" r:id="rId36" xr:uid="{B16F264A-0404-1E47-AC7B-2898F93925B7}"/>
-    <hyperlink ref="C38" r:id="rId37" xr:uid="{2F60B1C6-1590-FA42-8088-F70508BB1B6E}"/>
-    <hyperlink ref="C39" r:id="rId38" xr:uid="{007B0024-8C45-884B-94AA-1002459B034B}"/>
-    <hyperlink ref="C40" r:id="rId39" xr:uid="{4F65FC8A-4C13-AC42-A744-2E9BC53A30FC}"/>
-    <hyperlink ref="C41" r:id="rId40" xr:uid="{D3DE955B-43D0-054F-B926-FB03CA62B109}"/>
-    <hyperlink ref="C42" r:id="rId41" xr:uid="{2C604764-6CB2-E844-B6E5-A6E555DCE273}"/>
-    <hyperlink ref="C43" r:id="rId42" xr:uid="{13566D61-8EA1-5F4D-85F8-5CFFB01B935E}"/>
-    <hyperlink ref="C44" r:id="rId43" xr:uid="{BE2A6FD9-DC5C-F640-847C-B9DFFE1FBB39}"/>
-    <hyperlink ref="C45" r:id="rId44" xr:uid="{4C3DA420-966C-774F-8802-0EBC3ABE4016}"/>
-    <hyperlink ref="C46" r:id="rId45" xr:uid="{AB8F8534-6297-0C41-A3E6-EDE947967742}"/>
-    <hyperlink ref="C47" r:id="rId46" xr:uid="{5762E2B2-78EB-D241-B42E-F15523566E15}"/>
-    <hyperlink ref="C48" r:id="rId47" xr:uid="{F9A373C7-63F4-3B4D-AE37-D2980D8DAB2E}"/>
-    <hyperlink ref="C50" r:id="rId48" xr:uid="{DDD60544-6BD5-FE4D-BA67-F3438F7B6067}"/>
-    <hyperlink ref="C49" r:id="rId49" xr:uid="{B854AB59-57D5-F741-9CA3-630038480F13}"/>
-    <hyperlink ref="C53" r:id="rId50" xr:uid="{CB618DAF-CEA2-334D-BDEF-88A2974035C7}"/>
-    <hyperlink ref="C51" r:id="rId51" xr:uid="{529451F6-45AC-A644-AC4D-9D1337A50EE6}"/>
-    <hyperlink ref="C52" r:id="rId52" xr:uid="{01C85A55-2C64-4547-A29E-86FC11A4D774}"/>
-    <hyperlink ref="C54" r:id="rId53" xr:uid="{96D6A79A-DA38-F04F-9A4F-9531E98AC287}"/>
-    <hyperlink ref="C55" r:id="rId54" xr:uid="{A0876BC9-CE35-C144-B301-FB6C60B54356}"/>
-    <hyperlink ref="C56" r:id="rId55" xr:uid="{51B98318-899D-FD48-AD0B-642B6CCEC59F}"/>
-    <hyperlink ref="C57" r:id="rId56" xr:uid="{7686B834-B306-D74E-A513-8C288D691608}"/>
-    <hyperlink ref="C58" r:id="rId57" xr:uid="{CDB5E47F-FB83-6540-B3A6-B2AB1CF4AA6F}"/>
-    <hyperlink ref="C60" r:id="rId58" xr:uid="{E901C762-5EA0-1C46-B819-FA45DACCC29B}"/>
-    <hyperlink ref="C59" r:id="rId59" xr:uid="{2FD281AF-2188-8E4A-A4F7-0D9EAE7F9393}"/>
-    <hyperlink ref="C61" r:id="rId60" xr:uid="{2F9D69FF-CBFB-734E-9F40-DA351FADAFBA}"/>
-    <hyperlink ref="C62" r:id="rId61" xr:uid="{6C7F4A9C-D364-A144-B5FB-EA1668577004}"/>
-    <hyperlink ref="C63" r:id="rId62" xr:uid="{AB0031E2-E725-A146-8932-1E9CD49E3D9C}"/>
-    <hyperlink ref="C67" r:id="rId63" xr:uid="{3D6866E0-AC99-5C49-AD03-E77FC895E54B}"/>
-    <hyperlink ref="C64" r:id="rId64" xr:uid="{54487D76-C4F7-8C42-8B33-9FA9B16FA642}"/>
-    <hyperlink ref="C65" r:id="rId65" xr:uid="{3552050E-A192-CA41-B091-7C415450D223}"/>
-    <hyperlink ref="C66" r:id="rId66" xr:uid="{78A23032-CF5F-0842-A85A-D33126BA38A4}"/>
-    <hyperlink ref="C68" r:id="rId67" xr:uid="{39AD91F8-27C3-A14D-850F-A5E3812ED347}"/>
-    <hyperlink ref="C69" r:id="rId68" xr:uid="{308A730E-90FE-454F-9BDB-DF6F22045A35}"/>
-    <hyperlink ref="C70" r:id="rId69" xr:uid="{E0611B0E-7EB3-F546-A927-5E3CA02CBDC8}"/>
-    <hyperlink ref="C73" r:id="rId70" xr:uid="{48139188-43BA-5547-9AB9-0017F594BC55}"/>
-    <hyperlink ref="C71" r:id="rId71" xr:uid="{B1D90D64-2A87-7D40-B33B-D3EE397AAC6D}"/>
-    <hyperlink ref="C72" r:id="rId72" xr:uid="{0BF4D65A-F579-3E48-BD7B-858E4DD903D8}"/>
-    <hyperlink ref="C74" r:id="rId73" xr:uid="{3E2DF499-D764-F04A-B8C4-D566AAB484AF}"/>
-    <hyperlink ref="C75" r:id="rId74" xr:uid="{9FB1EDC1-0591-E943-A272-383542A5E4F7}"/>
-    <hyperlink ref="C76" r:id="rId75" xr:uid="{68405756-F780-394C-8A23-76CDEA9251E8}"/>
-    <hyperlink ref="C77" r:id="rId76" xr:uid="{D8F52D7D-FAA7-8949-920C-A6CC8F605E7B}"/>
-    <hyperlink ref="C78" r:id="rId77" xr:uid="{0F37E849-A76B-6C45-BB2C-FBDDADE5924A}"/>
-    <hyperlink ref="C79" r:id="rId78" xr:uid="{5AEBE584-8308-AC46-81E1-13B6DFD29028}"/>
-    <hyperlink ref="C80" r:id="rId79" xr:uid="{3312E3CA-9E78-8D4E-98A5-4CE85F73621A}"/>
-    <hyperlink ref="C81" r:id="rId80" xr:uid="{A5DCBC27-6C1E-3147-A8DD-8EC138CB970E}"/>
-    <hyperlink ref="C82" r:id="rId81" xr:uid="{19C9B0B1-6190-6544-ABD7-97E1DE8F389B}"/>
-    <hyperlink ref="C84" r:id="rId82" xr:uid="{312EC8CB-A58D-0944-BCAE-E0D8ADA03588}"/>
-    <hyperlink ref="C83" r:id="rId83" xr:uid="{D61051D5-CDFD-534E-9388-BC712D956B0C}"/>
-    <hyperlink ref="C86" r:id="rId84" xr:uid="{8D551D46-C8BC-524A-B78C-0423FE01E42C}"/>
-    <hyperlink ref="C85" r:id="rId85" xr:uid="{31560A24-20F5-4E4D-9B04-60D2C14BEF31}"/>
-    <hyperlink ref="C87" r:id="rId86" xr:uid="{F5CC44A4-098C-B742-814D-C3A130489199}"/>
-    <hyperlink ref="C88" r:id="rId87" xr:uid="{F4C02A42-7659-2C4D-A0A0-AFED22A3071D}"/>
-    <hyperlink ref="C89" r:id="rId88" xr:uid="{89774CCE-EFF2-5446-9D33-B39025F4A328}"/>
-    <hyperlink ref="C90" r:id="rId89" xr:uid="{11D46CB8-8B23-F841-BE5C-D94E0626C0AD}"/>
-    <hyperlink ref="C91" r:id="rId90" xr:uid="{A7250DF0-9B0C-7A4A-88BA-7C0B79387974}"/>
-    <hyperlink ref="C92" r:id="rId91" xr:uid="{4F1876B7-5DA8-0546-A12E-1574D12A5598}"/>
-    <hyperlink ref="C93" r:id="rId92" xr:uid="{4428663B-A783-0546-8C75-05A24F3A95FC}"/>
-    <hyperlink ref="C94" r:id="rId93" xr:uid="{4C989E5D-295F-814E-8041-F7FD75E30E47}"/>
-    <hyperlink ref="C95" r:id="rId94" xr:uid="{AB81B22C-A272-E741-A68D-6C7274E266CD}"/>
-    <hyperlink ref="C97" r:id="rId95" xr:uid="{68D0ED8B-64D5-0B42-BDD2-C31CD583C942}"/>
-    <hyperlink ref="C96" r:id="rId96" xr:uid="{5CBB78FD-DA99-E749-82AA-0C1ABF5DB2F3}"/>
-    <hyperlink ref="C98" r:id="rId97" xr:uid="{DB0778A7-C243-A34F-A076-D341F86E67A5}"/>
-    <hyperlink ref="C99" r:id="rId98" xr:uid="{FC634DCA-41AA-214A-B2D9-A0135E087044}"/>
-    <hyperlink ref="C100" r:id="rId99" xr:uid="{4A7EB823-9CD4-AF4A-965B-A699EAD713F7}"/>
-    <hyperlink ref="C101" r:id="rId100" xr:uid="{445AEDDD-343A-614A-80F5-4A8299826349}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{D12F1D2D-4B1F-9442-8230-BA093CCDA23F}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{FA3024EF-FFBD-684D-9906-53225CA54BB7}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{4FE93F76-11C2-634E-B1BA-33CD6EED3C4F}"/>
+    <hyperlink ref="D12" r:id="rId4" xr:uid="{0DE70282-1533-FB4C-B78F-7BE0837CF03F}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{2FE01F9A-75C7-EE45-9469-1989FC2664C1}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{5C5E2DBC-A8AD-2844-9409-F9591E3DA727}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{B2A6DD76-F50B-864A-BCA1-15F8CD8AD2F7}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{38D8F804-B45A-6F41-AB35-55FFD71423C7}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{3184A6BA-4C96-754E-B82D-4FF6352DAC7C}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{3EEA19BB-BEFA-E041-A042-A84DECF94176}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{0C3C1D74-1886-E948-8479-D03A38A04087}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{0D88BE8D-FCF7-3040-8284-06EB8E532A21}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{B177BDD6-35CA-AF4A-806D-E1566D9F25BB}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{D5461290-BDB0-4B4C-AC07-7BBEF6892BB5}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{484B8704-496B-2E48-885A-5472E9141AD4}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{EFFBA2DD-F5C7-4D42-8006-C5DB783D84E1}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{06E602B6-AA16-B448-BC4D-18D32CD932C7}"/>
+    <hyperlink ref="D27" r:id="rId18" xr:uid="{CA03CEA7-D903-0B47-BD15-0E012F5A8C55}"/>
+    <hyperlink ref="D26" r:id="rId19" xr:uid="{3507CF5C-F543-0F43-BEB0-DCA754D009BF}"/>
+    <hyperlink ref="D24" r:id="rId20" xr:uid="{4C82D90D-8FD6-2040-A1F0-96089A16509F}"/>
+    <hyperlink ref="D25" r:id="rId21" xr:uid="{32EB20C6-DC11-5040-B11B-6DCD9C5CDDA2}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{3287F51F-E3CA-284E-8EBB-980F59767731}"/>
+    <hyperlink ref="D22" r:id="rId23" xr:uid="{571A85DD-AD55-6E4C-AABC-2F061989418E}"/>
+    <hyperlink ref="D21" r:id="rId24" xr:uid="{3E840ED0-DB72-3D40-8F7A-7A636A18CFE2}"/>
+    <hyperlink ref="D20" r:id="rId25" xr:uid="{6B54AEE2-013B-4C44-83D0-7ACEA638D760}"/>
+    <hyperlink ref="D19" r:id="rId26" xr:uid="{E166F943-AD05-C644-ADFA-E6EABF1F4DD6}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{A87368AC-9E4A-C040-985C-E474B7165AC2}"/>
+    <hyperlink ref="D30" r:id="rId28" xr:uid="{0693A7AB-A5CC-CE44-A0A5-672D8C5E5CCB}"/>
+    <hyperlink ref="D29" r:id="rId29" xr:uid="{DB2CBE5D-C54C-9C4A-98CC-19C8994A1194}"/>
+    <hyperlink ref="D31" r:id="rId30" xr:uid="{6B30E3AF-1CF1-574A-B9FA-AA21C36DA4A4}"/>
+    <hyperlink ref="D32" r:id="rId31" xr:uid="{7103085F-DD81-3945-863D-D5FB32BDB2E1}"/>
+    <hyperlink ref="D33" r:id="rId32" xr:uid="{9D293948-3F61-6B42-A230-7F5AEC69950B}"/>
+    <hyperlink ref="D34" r:id="rId33" xr:uid="{274CB73F-F748-3E4C-87D9-3A18C2381AB8}"/>
+    <hyperlink ref="D36" r:id="rId34" xr:uid="{98178744-49F4-BE47-83D0-177CB7DD8461}"/>
+    <hyperlink ref="D35" r:id="rId35" xr:uid="{E2F229ED-615E-7F47-9665-16C479E0930F}"/>
+    <hyperlink ref="D37" r:id="rId36" xr:uid="{B16F264A-0404-1E47-AC7B-2898F93925B7}"/>
+    <hyperlink ref="D38" r:id="rId37" xr:uid="{2F60B1C6-1590-FA42-8088-F70508BB1B6E}"/>
+    <hyperlink ref="D39" r:id="rId38" xr:uid="{007B0024-8C45-884B-94AA-1002459B034B}"/>
+    <hyperlink ref="D40" r:id="rId39" xr:uid="{4F65FC8A-4C13-AC42-A744-2E9BC53A30FC}"/>
+    <hyperlink ref="D41" r:id="rId40" xr:uid="{D3DE955B-43D0-054F-B926-FB03CA62B109}"/>
+    <hyperlink ref="D42" r:id="rId41" xr:uid="{2C604764-6CB2-E844-B6E5-A6E555DCE273}"/>
+    <hyperlink ref="D43" r:id="rId42" xr:uid="{13566D61-8EA1-5F4D-85F8-5CFFB01B935E}"/>
+    <hyperlink ref="D44" r:id="rId43" xr:uid="{BE2A6FD9-DC5C-F640-847C-B9DFFE1FBB39}"/>
+    <hyperlink ref="D45" r:id="rId44" xr:uid="{4C3DA420-966C-774F-8802-0EBC3ABE4016}"/>
+    <hyperlink ref="D46" r:id="rId45" xr:uid="{AB8F8534-6297-0C41-A3E6-EDE947967742}"/>
+    <hyperlink ref="D47" r:id="rId46" xr:uid="{5762E2B2-78EB-D241-B42E-F15523566E15}"/>
+    <hyperlink ref="D48" r:id="rId47" xr:uid="{F9A373C7-63F4-3B4D-AE37-D2980D8DAB2E}"/>
+    <hyperlink ref="D50" r:id="rId48" xr:uid="{DDD60544-6BD5-FE4D-BA67-F3438F7B6067}"/>
+    <hyperlink ref="D49" r:id="rId49" xr:uid="{B854AB59-57D5-F741-9CA3-630038480F13}"/>
+    <hyperlink ref="D53" r:id="rId50" xr:uid="{CB618DAF-CEA2-334D-BDEF-88A2974035C7}"/>
+    <hyperlink ref="D51" r:id="rId51" xr:uid="{529451F6-45AC-A644-AC4D-9D1337A50EE6}"/>
+    <hyperlink ref="D52" r:id="rId52" xr:uid="{01C85A55-2C64-4547-A29E-86FC11A4D774}"/>
+    <hyperlink ref="D54" r:id="rId53" xr:uid="{96D6A79A-DA38-F04F-9A4F-9531E98AC287}"/>
+    <hyperlink ref="D55" r:id="rId54" xr:uid="{A0876BC9-CE35-C144-B301-FB6C60B54356}"/>
+    <hyperlink ref="D56" r:id="rId55" xr:uid="{51B98318-899D-FD48-AD0B-642B6CCEC59F}"/>
+    <hyperlink ref="D57" r:id="rId56" xr:uid="{7686B834-B306-D74E-A513-8C288D691608}"/>
+    <hyperlink ref="D58" r:id="rId57" xr:uid="{CDB5E47F-FB83-6540-B3A6-B2AB1CF4AA6F}"/>
+    <hyperlink ref="D60" r:id="rId58" xr:uid="{E901C762-5EA0-1C46-B819-FA45DACCC29B}"/>
+    <hyperlink ref="D59" r:id="rId59" xr:uid="{2FD281AF-2188-8E4A-A4F7-0D9EAE7F9393}"/>
+    <hyperlink ref="D61" r:id="rId60" xr:uid="{2F9D69FF-CBFB-734E-9F40-DA351FADAFBA}"/>
+    <hyperlink ref="D62" r:id="rId61" xr:uid="{6C7F4A9C-D364-A144-B5FB-EA1668577004}"/>
+    <hyperlink ref="D63" r:id="rId62" xr:uid="{AB0031E2-E725-A146-8932-1E9CD49E3D9C}"/>
+    <hyperlink ref="D67" r:id="rId63" xr:uid="{3D6866E0-AC99-5C49-AD03-E77FC895E54B}"/>
+    <hyperlink ref="D64" r:id="rId64" xr:uid="{54487D76-C4F7-8C42-8B33-9FA9B16FA642}"/>
+    <hyperlink ref="D65" r:id="rId65" xr:uid="{3552050E-A192-CA41-B091-7C415450D223}"/>
+    <hyperlink ref="D66" r:id="rId66" xr:uid="{78A23032-CF5F-0842-A85A-D33126BA38A4}"/>
+    <hyperlink ref="D68" r:id="rId67" xr:uid="{39AD91F8-27C3-A14D-850F-A5E3812ED347}"/>
+    <hyperlink ref="D69" r:id="rId68" xr:uid="{308A730E-90FE-454F-9BDB-DF6F22045A35}"/>
+    <hyperlink ref="D70" r:id="rId69" xr:uid="{E0611B0E-7EB3-F546-A927-5E3CA02CBDC8}"/>
+    <hyperlink ref="D73" r:id="rId70" xr:uid="{48139188-43BA-5547-9AB9-0017F594BC55}"/>
+    <hyperlink ref="D71" r:id="rId71" xr:uid="{B1D90D64-2A87-7D40-B33B-D3EE397AAC6D}"/>
+    <hyperlink ref="D72" r:id="rId72" xr:uid="{0BF4D65A-F579-3E48-BD7B-858E4DD903D8}"/>
+    <hyperlink ref="D74" r:id="rId73" xr:uid="{3E2DF499-D764-F04A-B8C4-D566AAB484AF}"/>
+    <hyperlink ref="D75" r:id="rId74" xr:uid="{9FB1EDC1-0591-E943-A272-383542A5E4F7}"/>
+    <hyperlink ref="D76" r:id="rId75" xr:uid="{68405756-F780-394C-8A23-76CDEA9251E8}"/>
+    <hyperlink ref="D77" r:id="rId76" xr:uid="{D8F52D7D-FAA7-8949-920C-A6CC8F605E7B}"/>
+    <hyperlink ref="D78" r:id="rId77" xr:uid="{0F37E849-A76B-6C45-BB2C-FBDDADE5924A}"/>
+    <hyperlink ref="D79" r:id="rId78" xr:uid="{5AEBE584-8308-AC46-81E1-13B6DFD29028}"/>
+    <hyperlink ref="D80" r:id="rId79" xr:uid="{3312E3CA-9E78-8D4E-98A5-4CE85F73621A}"/>
+    <hyperlink ref="D81" r:id="rId80" xr:uid="{A5DCBC27-6C1E-3147-A8DD-8EC138CB970E}"/>
+    <hyperlink ref="D82" r:id="rId81" xr:uid="{19C9B0B1-6190-6544-ABD7-97E1DE8F389B}"/>
+    <hyperlink ref="D84" r:id="rId82" xr:uid="{312EC8CB-A58D-0944-BCAE-E0D8ADA03588}"/>
+    <hyperlink ref="D83" r:id="rId83" xr:uid="{D61051D5-CDFD-534E-9388-BC712D956B0C}"/>
+    <hyperlink ref="D86" r:id="rId84" xr:uid="{8D551D46-C8BC-524A-B78C-0423FE01E42C}"/>
+    <hyperlink ref="D85" r:id="rId85" xr:uid="{31560A24-20F5-4E4D-9B04-60D2C14BEF31}"/>
+    <hyperlink ref="D87" r:id="rId86" xr:uid="{F5CC44A4-098C-B742-814D-C3A130489199}"/>
+    <hyperlink ref="D88" r:id="rId87" xr:uid="{F4C02A42-7659-2C4D-A0A0-AFED22A3071D}"/>
+    <hyperlink ref="D89" r:id="rId88" xr:uid="{89774CCE-EFF2-5446-9D33-B39025F4A328}"/>
+    <hyperlink ref="D90" r:id="rId89" xr:uid="{11D46CB8-8B23-F841-BE5C-D94E0626C0AD}"/>
+    <hyperlink ref="D91" r:id="rId90" xr:uid="{A7250DF0-9B0C-7A4A-88BA-7C0B79387974}"/>
+    <hyperlink ref="D92" r:id="rId91" xr:uid="{4F1876B7-5DA8-0546-A12E-1574D12A5598}"/>
+    <hyperlink ref="D93" r:id="rId92" xr:uid="{4428663B-A783-0546-8C75-05A24F3A95FC}"/>
+    <hyperlink ref="D94" r:id="rId93" xr:uid="{4C989E5D-295F-814E-8041-F7FD75E30E47}"/>
+    <hyperlink ref="D95" r:id="rId94" xr:uid="{AB81B22C-A272-E741-A68D-6C7274E266CD}"/>
+    <hyperlink ref="D97" r:id="rId95" xr:uid="{68D0ED8B-64D5-0B42-BDD2-C31CD583C942}"/>
+    <hyperlink ref="D96" r:id="rId96" xr:uid="{5CBB78FD-DA99-E749-82AA-0C1ABF5DB2F3}"/>
+    <hyperlink ref="D98" r:id="rId97" xr:uid="{DB0778A7-C243-A34F-A076-D341F86E67A5}"/>
+    <hyperlink ref="D99" r:id="rId98" xr:uid="{FC634DCA-41AA-214A-B2D9-A0135E087044}"/>
+    <hyperlink ref="D100" r:id="rId99" xr:uid="{4A7EB823-9CD4-AF4A-965B-A699EAD713F7}"/>
+    <hyperlink ref="D101" r:id="rId100" xr:uid="{445AEDDD-343A-614A-80F5-4A8299826349}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>